<commit_message>
Proyecto Concluido Con Exito :)
</commit_message>
<xml_diff>
--- a/diagrama de pareto para la empresa 11062024.xlsx
+++ b/diagrama de pareto para la empresa 11062024.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeta\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeta\Desktop\cotizaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2253E039-8D10-4C7D-8F3D-8C0D4A900F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1038E0C-065A-452C-88DC-ACF841F0567D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7413B629-842F-4DC1-B58D-C342CBBDE5DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,13 +54,13 @@
     <t xml:space="preserve">Comunicación Interna	</t>
   </si>
   <si>
-    <t xml:space="preserve">Sistema de cotizacion desfasado </t>
-  </si>
-  <si>
     <t>Capacitación y Desarrollo Profesional</t>
   </si>
   <si>
     <t>Otros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema de cotizacion manual </t>
   </si>
 </sst>
 </file>
@@ -320,7 +320,7 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Sistema de cotizacion desfasado </c:v>
+                  <c:v>Sistema de cotizacion manual </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Satisfacción con la Precisión de las Cotizaciones	</c:v>
@@ -556,7 +556,7 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Sistema de cotizacion desfasado </c:v>
+                  <c:v>Sistema de cotizacion manual </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Satisfacción con la Precisión de las Cotizaciones	</c:v>
@@ -1847,7 +1847,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>50</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
         <v>15</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="8">
         <v>8</v>

</xml_diff>